<commit_message>
2nd Commit, with completed sample code for reading all the data in the excel sheetand print it in the console.
</commit_message>
<xml_diff>
--- a/src/test/java/testData/dataSheet.xlsx
+++ b/src/test/java/testData/dataSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arunp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backup\Selenium - Workspace\IdeaProjects\ApachePOISimple\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277B439D-8C4B-46B5-9BBF-52A11275093C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955B9189-3BC8-4F9A-BDA7-629D4ECD8268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>